<commit_message>
updated timings and configured npsim to run method 2 simulations
</commit_message>
<xml_diff>
--- a/beatthestreak/times/2010, 2009, 300, 300D,sM=1 Times.xlsx
+++ b/beatthestreak/times/2010, 2009, 300, 300D,sM=1 Times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Update copy_bot removed" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="NewDateBaseline" sheetId="3" r:id="rId3"/>
     <sheet name="Removed Reporting" sheetId="4" r:id="rId4"/>
     <sheet name="Removed Asserts" sheetId="5" r:id="rId5"/>
+    <sheet name="cdid_start" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="20">
   <si>
     <t>T1</t>
   </si>
@@ -80,6 +81,9 @@
   </si>
   <si>
     <t>Removed all assert statements</t>
+  </si>
+  <si>
+    <t>Implemented c_did_start function</t>
   </si>
 </sst>
 </file>
@@ -143,8 +147,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -164,17 +170,19 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1136,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1233,6 +1241,165 @@
       <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>9.1333333333333336E-2</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.863</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.861</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.869</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8643333333333334</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666666E-3</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.014</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="E2" s="4">
+        <f>AVERAGE(B2:D2)</f>
+        <v>0.97000000000000008</v>
+      </c>
+      <c r="F2" s="4">
+        <f>('Removed Asserts'!E2-cdid_start!E2)/'Removed Asserts'!E2</f>
+        <v>0.22688629117959619</v>
+      </c>
+      <c r="G2" s="5">
+        <v>41821</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.873</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E6" si="0">AVERAGE(B3:D3)</f>
+        <v>0.8736666666666667</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>8.0666666666666664E-2</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>

</xml_diff>